<commit_message>
Read from email logic added
</commit_message>
<xml_diff>
--- a/InputData/Sample_backup.xlsx
+++ b/InputData/Sample_backup.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shreyas.Risodkar\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/shreyas_risodkar_uipath_com/Documents/UiPath_LearningDocs/Code/CM Sandbox code/CM_Demo/InputData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8353DD51-53F7-4DAC-84B7-FB7020E05273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{4E4AC13E-CE6B-4B5F-91C8-B542379C642E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85D9A795-6393-4DA1-BAAF-2A3152925A32}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="120" windowWidth="19120" windowHeight="10220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028" iterateDelta="1E-4"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
   <si>
     <t>Comment ID</t>
   </si>
@@ -65,9 +66,6 @@
     <t>A1</t>
   </si>
   <si>
-    <t>lesley20@mitchell.com</t>
-  </si>
-  <si>
     <t>berniece.heller@schamberger.org</t>
   </si>
   <si>
@@ -77,14 +75,28 @@
     <t>Bronze</t>
   </si>
   <si>
-    <t>2023-06-19T10:32:12Z</t>
-  </si>
-  <si>
-    <t>To berniece.heller@schamberger.org
-Photo advertised shows the le Pedrera lit up at night We visited the roof top bar to see le Pedrera lit up at night and it is blocked to be unable to see it</t>
-  </si>
-  <si>
-    <t>Pedera Review new1</t>
+    <t>leslei201@mitchell.com</t>
+  </si>
+  <si>
+    <t>2023-06-19T10:33:12Z</t>
+  </si>
+  <si>
+    <t>Expected better service again</t>
+  </si>
+  <si>
+    <t>Room was a bit dark, facilities could have been much better. Will not visit again.</t>
+  </si>
+  <si>
+    <t>Home Insurance Claim</t>
+  </si>
+  <si>
+    <t>I would like to file a claim for earthquake damage to my home.</t>
+  </si>
+  <si>
+    <t>underwriter@insurer.com</t>
+  </si>
+  <si>
+    <t>amber@customer.com</t>
   </si>
 </sst>
 </file>
@@ -493,42 +505,144 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="71.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="D2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
       </c>
       <c r="G2" t="s">
         <v>13</v>
       </c>
       <c r="H2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{2D7FD4DC-74BE-4429-8B57-8A7C24782351}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{1A08237D-0664-403B-B04F-F6FAD7CE5BFA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB23DEF0-F8DE-4EB0-9B3F-4CB4DEAC5BAC}">
+  <dimension ref="A2:H8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="A5:H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="72" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D5" r:id="rId1" xr:uid="{D0C4B39F-DF3B-479D-AB03-1001A4A1CC61}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100286A0E83FB7D6A4FABC39B8DA48BB7BE" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f761d087c8e1ac2be2355b6e56f2ee3e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6ffa1282-9dca-4a98-9d83-2f99b06c1687" xmlns:ns3="0b1013c3-c8b1-4041-81aa-a320da6bb7e1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="498c28b125ae3f15bb9bc01cc780facc" ns2:_="" ns3:_="">
     <xsd:import namespace="6ffa1282-9dca-4a98-9d83-2f99b06c1687"/>
@@ -699,7 +813,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -708,13 +822,16 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25629161-0555-4703-A291-B0A1BC136144}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E76E2E1-2277-4F2F-9E98-7E53CC615D36}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -733,19 +850,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52C71334-DA6B-480B-AC63-09BC4D870E08}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25629161-0555-4703-A291-B0A1BC136144}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>